<commit_message>
cosas de la dataBASE
</commit_message>
<xml_diff>
--- a/laliga/barcelona/barcelona.xlsx
+++ b/laliga/barcelona/barcelona.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomip\OneDrive\Documentos\pucelale\pucelale.local\laliga\barcelona\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC972683-9E62-4A38-86E7-E54DCEC32A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FD70BF-0DD7-4DC7-B8B3-E2E240ACB72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{6F209D07-E2EA-4A00-B580-60A30F1948D5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6F209D07-E2EA-4A00-B580-60A30F1948D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="179">
   <si>
     <t>Jugador</t>
   </si>
@@ -65,42 +65,27 @@
     <t>España</t>
   </si>
   <si>
-    <t>PT</t>
-  </si>
-  <si>
     <t>Dani Alves</t>
   </si>
   <si>
     <t>Brasil</t>
   </si>
   <si>
-    <t>LD</t>
-  </si>
-  <si>
     <t>Eric Abidal</t>
   </si>
   <si>
     <t>Francia</t>
   </si>
   <si>
-    <t>LI</t>
-  </si>
-  <si>
     <t>Carles Puyol</t>
   </si>
   <si>
-    <t>DFC</t>
-  </si>
-  <si>
     <t>Gerard Piqué</t>
   </si>
   <si>
     <t>Xavi Hernández</t>
   </si>
   <si>
-    <t>MCD</t>
-  </si>
-  <si>
     <t>Yaya Touré</t>
   </si>
   <si>
@@ -110,33 +95,21 @@
     <t>Andrés Iniesta</t>
   </si>
   <si>
-    <t>MP</t>
-  </si>
-  <si>
     <t>Samuel Eto'o</t>
   </si>
   <si>
     <t>Camerun</t>
   </si>
   <si>
-    <t>DC</t>
-  </si>
-  <si>
     <t>Leo Messi</t>
   </si>
   <si>
     <t>Argentina</t>
   </si>
   <si>
-    <t>ED</t>
-  </si>
-  <si>
     <t>Thierry Henry</t>
   </si>
   <si>
-    <t>EI</t>
-  </si>
-  <si>
     <t>Jose Pinto</t>
   </si>
   <si>
@@ -591,6 +564,18 @@
   </si>
   <si>
     <t>Pau Victor</t>
+  </si>
+  <si>
+    <t>Centrocampista</t>
+  </si>
+  <si>
+    <t>Defensa</t>
+  </si>
+  <si>
+    <t>Portero</t>
+  </si>
+  <si>
+    <t>Atacante</t>
   </si>
 </sst>
 </file>
@@ -626,9 +611,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,33 +949,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{328909AE-6509-4DD9-BC7D-402A6B236C72}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1003,7 +988,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1017,13 +1002,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1037,13 +1022,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1057,13 +1042,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -1077,13 +1062,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1097,13 +1082,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1117,13 +1102,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1137,13 +1122,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -1157,13 +1142,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -1177,13 +1162,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -1197,13 +1182,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D12">
         <v>9</v>
@@ -1217,13 +1202,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -1237,13 +1222,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>178</v>
       </c>
       <c r="D14">
         <v>14</v>
@@ -1257,13 +1242,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>178</v>
       </c>
       <c r="D15">
         <v>9</v>
@@ -1277,13 +1262,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1297,13 +1282,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D17">
         <v>7</v>
@@ -1317,13 +1302,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D18">
         <v>24</v>
@@ -1337,13 +1322,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D19">
         <v>18</v>
@@ -1357,13 +1342,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D20">
         <v>21</v>
@@ -1377,13 +1362,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="D21">
         <v>16</v>
@@ -1397,13 +1382,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -1417,13 +1402,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D23">
         <v>29</v>
@@ -1437,13 +1422,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D24">
         <v>15</v>
@@ -1457,13 +1442,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D25">
         <v>11</v>
@@ -1477,13 +1462,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="D26">
         <v>25</v>
@@ -1497,13 +1482,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="D27">
         <v>19</v>
@@ -1517,13 +1502,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D28">
         <v>12</v>
@@ -1537,13 +1522,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D29">
         <v>9</v>
@@ -1557,13 +1542,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D30">
         <v>21</v>
@@ -1577,13 +1562,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="D31">
         <v>13</v>
@@ -1597,13 +1582,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D32">
         <v>11</v>
@@ -1617,13 +1602,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D33">
         <v>7</v>
@@ -1637,13 +1622,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -1657,13 +1642,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D35">
         <v>7</v>
@@ -1677,13 +1662,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="D36">
         <v>22</v>
@@ -1697,13 +1682,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D37">
         <v>8</v>
@@ -1717,13 +1702,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D38">
         <v>24</v>
@@ -1737,13 +1722,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -1757,13 +1742,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>178</v>
       </c>
       <c r="D40">
         <v>19</v>
@@ -1777,13 +1762,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D41">
         <v>6</v>
@@ -1797,13 +1782,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="D42">
         <v>25</v>
@@ -1817,13 +1802,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D43">
         <v>17</v>
@@ -1837,13 +1822,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D44">
         <v>23</v>
@@ -1857,13 +1842,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>31</v>
+        <v>178</v>
       </c>
       <c r="D45">
         <v>11</v>
@@ -1877,13 +1862,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D46">
         <v>6</v>
@@ -1897,13 +1882,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="D47">
         <v>13</v>
@@ -1917,13 +1902,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>31</v>
+        <v>178</v>
       </c>
       <c r="D48">
         <v>20</v>
@@ -1937,13 +1922,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D49">
         <v>15</v>
@@ -1957,13 +1942,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D50">
         <v>2</v>
@@ -1977,13 +1962,13 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B51" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -1997,13 +1982,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D52">
         <v>8</v>
@@ -2017,13 +2002,13 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="D53">
         <v>21</v>
@@ -2037,13 +2022,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C54" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D54">
         <v>14</v>
@@ -2057,13 +2042,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C55" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D55">
         <v>9</v>
@@ -2077,13 +2062,13 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C56" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D56">
         <v>10</v>
@@ -2097,13 +2082,13 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D57">
         <v>17</v>
@@ -2117,13 +2102,13 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C58" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D58">
         <v>24</v>
@@ -2137,13 +2122,13 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D59">
         <v>19</v>
@@ -2157,13 +2142,13 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="D60">
         <v>25</v>
@@ -2177,13 +2162,13 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -2197,13 +2182,13 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B62" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="D62">
         <v>19</v>
@@ -2217,13 +2202,13 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D63">
         <v>6</v>
@@ -2237,13 +2222,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B64" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C64" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D64">
         <v>21</v>
@@ -2257,13 +2242,13 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B65" t="s">
         <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D65">
         <v>22</v>
@@ -2277,13 +2262,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C66" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="D66">
         <v>13</v>
@@ -2297,13 +2282,13 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D67">
         <v>14</v>
@@ -2317,13 +2302,13 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>31</v>
+        <v>178</v>
       </c>
       <c r="D68">
         <v>16</v>
@@ -2337,13 +2322,13 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D69">
         <v>12</v>
@@ -2357,13 +2342,13 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D70">
         <v>16</v>
@@ -2377,13 +2362,13 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B71" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C71" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D71">
         <v>17</v>
@@ -2397,13 +2382,13 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
       </c>
       <c r="C72" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D72">
         <v>5</v>
@@ -2417,13 +2402,13 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D73">
         <v>15</v>
@@ -2437,13 +2422,13 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C74" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D74">
         <v>19</v>
@@ -2457,13 +2442,13 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B75" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C75" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D75">
         <v>19</v>
@@ -2477,13 +2462,13 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B76" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C76" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D76">
         <v>24</v>
@@ -2497,13 +2482,13 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B77" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C77" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D77">
         <v>7</v>
@@ -2517,13 +2502,13 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B78" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C78" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D78">
         <v>16</v>
@@ -2537,13 +2522,13 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="D79">
         <v>3</v>
@@ -2557,13 +2542,13 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B80" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C80" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D80">
         <v>7</v>
@@ -2577,13 +2562,13 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C81" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D81">
         <v>24</v>
@@ -2597,13 +2582,13 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D82">
         <v>6</v>
@@ -2617,13 +2602,13 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" t="s">
         <v>9</v>
       </c>
-      <c r="B83" t="s">
-        <v>10</v>
-      </c>
       <c r="C83" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D83">
         <v>8</v>
@@ -2637,13 +2622,13 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B84" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C84" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D84">
         <v>4</v>
@@ -2657,13 +2642,13 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
       </c>
       <c r="C85" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D85">
         <v>5</v>
@@ -2677,13 +2662,13 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B86" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C86" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D86">
         <v>22</v>
@@ -2697,13 +2682,13 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B87" t="s">
         <v>7</v>
       </c>
       <c r="C87" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D87">
         <v>11</v>
@@ -2717,13 +2702,13 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B88" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C88" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="D88">
         <v>24</v>
@@ -2737,13 +2722,13 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B89" t="s">
         <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D89">
         <v>27</v>
@@ -2757,13 +2742,13 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B90" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C90" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D90">
         <v>11</v>
@@ -2777,13 +2762,13 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B91" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C91" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D91">
         <v>12</v>
@@ -2797,13 +2782,13 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="D92">
         <v>13</v>
@@ -2817,13 +2802,13 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D93">
         <v>14</v>
@@ -2837,13 +2822,13 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B94" t="s">
         <v>7</v>
       </c>
       <c r="C94" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D94">
         <v>14</v>
@@ -2857,13 +2842,13 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B95" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C95" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D95">
         <v>15</v>
@@ -2877,13 +2862,13 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B96" t="s">
         <v>7</v>
       </c>
       <c r="C96" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D96">
         <v>6</v>
@@ -2897,13 +2882,13 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B97" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C97" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D97">
         <v>17</v>
@@ -2917,13 +2902,13 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B98" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C98" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D98">
         <v>8</v>
@@ -2937,13 +2922,13 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B99" t="s">
         <v>7</v>
       </c>
       <c r="C99" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D99">
         <v>27</v>
@@ -2957,13 +2942,13 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B100" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D100">
         <v>19</v>
@@ -2977,13 +2962,13 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B101" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C101" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D101">
         <v>17</v>
@@ -2997,13 +2982,13 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B102" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C102" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D102">
         <v>17</v>
@@ -3017,13 +3002,13 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B103" t="s">
         <v>7</v>
       </c>
       <c r="C103" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D103">
         <v>7</v>
@@ -3037,13 +3022,13 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B104" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C104" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D104">
         <v>19</v>
@@ -3057,13 +3042,13 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B105" t="s">
         <v>7</v>
       </c>
       <c r="C105" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D105">
         <v>8</v>
@@ -3077,13 +3062,13 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B106" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C106" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D106">
         <v>14</v>
@@ -3097,13 +3082,13 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B107" t="s">
         <v>7</v>
       </c>
       <c r="C107" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D107">
         <v>22</v>
@@ -3117,13 +3102,13 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B108" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C108" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D108">
         <v>22</v>
@@ -3137,13 +3122,13 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B109" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C109" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D109">
         <v>23</v>
@@ -3157,13 +3142,13 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B110" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C110" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D110">
         <v>9</v>
@@ -3177,13 +3162,13 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B111" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C111" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D111">
         <v>17</v>
@@ -3197,13 +3182,13 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B112" t="s">
         <v>7</v>
       </c>
       <c r="C112" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D112">
         <v>29</v>
@@ -3217,13 +3202,13 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B113" t="s">
         <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>31</v>
+        <v>178</v>
       </c>
       <c r="D113">
         <v>10</v>
@@ -3237,13 +3222,13 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B114" t="s">
         <v>7</v>
       </c>
       <c r="C114" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="D114">
         <v>18</v>
@@ -3257,13 +3242,13 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B115" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C115" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D115">
         <v>19</v>
@@ -3277,13 +3262,13 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B116" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C116" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D116">
         <v>11</v>
@@ -3297,13 +3282,13 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B117" t="s">
         <v>7</v>
       </c>
       <c r="C117" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="D117">
         <v>13</v>
@@ -3317,13 +3302,13 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B118" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C118" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D118">
         <v>14</v>
@@ -3337,13 +3322,13 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B119" t="s">
         <v>7</v>
       </c>
       <c r="C119" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D119">
         <v>14</v>
@@ -3357,13 +3342,13 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B120" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C120" t="s">
-        <v>31</v>
+        <v>178</v>
       </c>
       <c r="D120">
         <v>16</v>
@@ -3377,13 +3362,13 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B121" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C121" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D121">
         <v>15</v>
@@ -3397,13 +3382,13 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B122" t="s">
         <v>7</v>
       </c>
       <c r="C122" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="D122">
         <v>17</v>
@@ -3417,13 +3402,13 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B123" t="s">
         <v>7</v>
       </c>
       <c r="C123" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D123">
         <v>18</v>
@@ -3437,13 +3422,13 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B124" t="s">
         <v>7</v>
       </c>
       <c r="C124" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D124">
         <v>16</v>
@@ -3457,13 +3442,13 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B125" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C125" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D125">
         <v>19</v>
@@ -3477,13 +3462,13 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B126" t="s">
         <v>7</v>
       </c>
       <c r="C126" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D126">
         <v>20</v>
@@ -3497,13 +3482,13 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B127" t="s">
         <v>7</v>
       </c>
       <c r="C127" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D127">
         <v>17</v>
@@ -3517,13 +3502,13 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B128" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C128" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D128">
         <v>22</v>
@@ -3537,13 +3522,13 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B129" t="s">
         <v>7</v>
       </c>
       <c r="C129" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D129">
         <v>18</v>
@@ -3557,13 +3542,13 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B130" t="s">
         <v>7</v>
       </c>
       <c r="C130" t="s">
-        <v>29</v>
+        <v>178</v>
       </c>
       <c r="D130">
         <v>19</v>
@@ -3577,13 +3562,13 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B131" t="s">
         <v>7</v>
       </c>
       <c r="C131" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="D131">
         <v>20</v>
@@ -3597,13 +3582,13 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B132" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C132" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D132">
         <v>21</v>
@@ -3617,13 +3602,13 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B133" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C133" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D133">
         <v>23</v>
@@ -3637,13 +3622,13 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B134" t="s">
         <v>7</v>
       </c>
       <c r="C134" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="D134">
         <v>24</v>
@@ -3657,13 +3642,13 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B135" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C135" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="D135">
         <v>25</v>
@@ -3677,13 +3662,13 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B136" t="s">
         <v>7</v>
       </c>
       <c r="C136" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D136">
         <v>32</v>
@@ -3697,13 +3682,13 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B137" t="s">
         <v>7</v>
       </c>
       <c r="C137" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="D137">
         <v>35</v>

</xml_diff>